<commit_message>
to implement cross, elitism
</commit_message>
<xml_diff>
--- a/csv/visual.xlsx
+++ b/csv/visual.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\vet-css\csv\"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="199">
   <si>
     <t>John</t>
   </si>
@@ -560,13 +560,85 @@
   </si>
   <si>
     <t>key: 21 of child value scID: 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t xml:space="preserve">Room 2 </t>
+  </si>
+  <si>
+    <t>CANTEEN</t>
+  </si>
+  <si>
+    <t>1MATH101</t>
+  </si>
+  <si>
+    <t>3ENGL101</t>
+  </si>
+  <si>
+    <t>x= 0 key: 77 matingPoolFrequency: 33</t>
+  </si>
+  <si>
+    <t>x= 1 key: 7 matingPoolFrequency: 20</t>
+  </si>
+  <si>
+    <t>x= 2 key: 52 matingPoolFrequency: 17</t>
+  </si>
+  <si>
+    <t>x= 3 key: 31 matingPoolFrequency: 14</t>
+  </si>
+  <si>
+    <t>x= 4 key: 5 matingPoolFrequency: 13</t>
+  </si>
+  <si>
+    <t>x= 5 key: 6 matingPoolFrequency: 11</t>
+  </si>
+  <si>
+    <t>x= 6 key: 2 matingPoolFrequency: 10</t>
+  </si>
+  <si>
+    <t>x= 7 key: 1 matingPoolFrequency: 9</t>
+  </si>
+  <si>
+    <t>x= 8 key: 8 matingPoolFrequency: 8</t>
+  </si>
+  <si>
+    <t>x= 9 key: 0 matingPoolFrequency: 8</t>
+  </si>
+  <si>
+    <t>x= 10 key: 14 matingPoolFrequency: 7</t>
+  </si>
+  <si>
+    <t>x= 11 key: 26 matingPoolFrequency: 7</t>
+  </si>
+  <si>
+    <t>x= 12 key: 9 matingPoolFrequency: 6</t>
+  </si>
+  <si>
+    <t>x= 13 key: 25 matingPoolFrequency: 6</t>
+  </si>
+  <si>
+    <t>x= 14 key: 11 matingPoolFrequency: 5</t>
+  </si>
+  <si>
+    <t>x= 15 key: 18 matingPoolFrequency: 5</t>
+  </si>
+  <si>
+    <t>Size matingPool :  179</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1001,7 +1073,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1418,6 +1490,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1436,9 +1533,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1476,7 +1571,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{26416ADD-37C9-4027-A250-3B5E8C02049A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26416ADD-37C9-4027-A250-3B5E8C02049A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1809,11 +1904,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AH50"/>
   <sheetViews>
-    <sheetView topLeftCell="E21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N52" sqref="N52"/>
+    <sheetView topLeftCell="AH11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15:AH31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -1829,7 +1924,7 @@
     <col min="15" max="34" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:34" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="60">
       <c r="G3" s="1" t="s">
         <v>77</v>
       </c>
@@ -1859,7 +1954,7 @@
       </c>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1901,7 +1996,7 @@
       </c>
       <c r="P4" s="5"/>
     </row>
-    <row r="5" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="30">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1943,7 +2038,7 @@
       </c>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1985,7 +2080,7 @@
       </c>
       <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" ht="30">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2027,7 +2122,7 @@
       </c>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" ht="30">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2069,7 +2164,7 @@
       </c>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" ht="30">
       <c r="G9" s="1">
         <v>6</v>
       </c>
@@ -2099,7 +2194,7 @@
       </c>
       <c r="P9" s="2"/>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2116,7 +2211,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2133,7 +2228,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34" ht="15.75" thickBot="1">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2150,7 +2245,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34">
       <c r="A15">
         <v>3</v>
       </c>
@@ -2166,36 +2261,36 @@
       <c r="E15" t="s">
         <v>19</v>
       </c>
-      <c r="O15" s="140" t="s">
+      <c r="O15" s="149" t="s">
         <v>25</v>
       </c>
-      <c r="P15" s="141"/>
-      <c r="Q15" s="141"/>
-      <c r="R15" s="141"/>
-      <c r="S15" s="142"/>
-      <c r="T15" s="143" t="s">
+      <c r="P15" s="150"/>
+      <c r="Q15" s="150"/>
+      <c r="R15" s="150"/>
+      <c r="S15" s="151"/>
+      <c r="T15" s="152" t="s">
         <v>72</v>
       </c>
-      <c r="U15" s="144"/>
-      <c r="V15" s="144"/>
-      <c r="W15" s="144"/>
-      <c r="X15" s="145"/>
-      <c r="Y15" s="140" t="s">
+      <c r="U15" s="153"/>
+      <c r="V15" s="153"/>
+      <c r="W15" s="153"/>
+      <c r="X15" s="154"/>
+      <c r="Y15" s="149" t="s">
         <v>70</v>
       </c>
-      <c r="Z15" s="141"/>
-      <c r="AA15" s="141"/>
-      <c r="AB15" s="141"/>
-      <c r="AC15" s="142"/>
-      <c r="AD15" s="143" t="s">
+      <c r="Z15" s="150"/>
+      <c r="AA15" s="150"/>
+      <c r="AB15" s="150"/>
+      <c r="AC15" s="151"/>
+      <c r="AD15" s="152" t="s">
         <v>71</v>
       </c>
-      <c r="AE15" s="144"/>
-      <c r="AF15" s="144"/>
-      <c r="AG15" s="144"/>
-      <c r="AH15" s="145"/>
-    </row>
-    <row r="16" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE15" s="153"/>
+      <c r="AF15" s="153"/>
+      <c r="AG15" s="153"/>
+      <c r="AH15" s="154"/>
+    </row>
+    <row r="16" spans="1:34" ht="15.75" thickBot="1">
       <c r="J16" s="2" t="s">
         <v>54</v>
       </c>
@@ -2268,7 +2363,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" ht="30">
       <c r="J17" s="3">
         <f>QUOTIENT(L17,5)+1</f>
         <v>1</v>
@@ -2359,7 +2454,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" ht="30">
       <c r="J18" s="3">
         <f t="shared" ref="J18:J31" si="4">QUOTIENT(L18,5)+1</f>
         <v>1</v>
@@ -2446,7 +2541,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -2548,7 +2643,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" ht="30">
       <c r="A20">
         <v>1</v>
       </c>
@@ -2653,7 +2748,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:34" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:34" ht="30.75" thickBot="1">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2758,7 +2853,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" ht="30">
       <c r="H22">
         <v>0</v>
       </c>
@@ -2851,7 +2946,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" ht="30">
       <c r="H23">
         <v>7</v>
       </c>
@@ -2942,7 +3037,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" ht="30">
       <c r="H24">
         <v>10</v>
       </c>
@@ -3032,7 +3127,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -3137,7 +3232,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:34" ht="15.75" thickBot="1">
       <c r="A26">
         <v>1</v>
       </c>
@@ -3239,7 +3334,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" ht="30">
       <c r="A27">
         <v>2</v>
       </c>
@@ -3343,7 +3438,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" ht="30">
       <c r="A28">
         <v>3</v>
       </c>
@@ -3445,7 +3540,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34">
       <c r="A29">
         <v>4</v>
       </c>
@@ -3547,7 +3642,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34">
       <c r="J30" s="3">
         <f t="shared" si="4"/>
         <v>3</v>
@@ -3632,7 +3727,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:34" ht="15.75" thickBot="1">
       <c r="J31" s="3">
         <f t="shared" si="4"/>
         <v>3</v>
@@ -3717,7 +3812,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34">
       <c r="O32" s="23"/>
       <c r="P32" s="23"/>
       <c r="Q32" s="23"/>
@@ -3739,7 +3834,7 @@
       <c r="AG32" s="23"/>
       <c r="AH32" s="23"/>
     </row>
-    <row r="33" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:34">
       <c r="C33" t="s">
         <v>45</v>
       </c>
@@ -3764,7 +3859,7 @@
       <c r="AG33" s="23"/>
       <c r="AH33" s="23"/>
     </row>
-    <row r="34" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:34">
       <c r="C34" t="s">
         <v>46</v>
       </c>
@@ -3797,7 +3892,7 @@
       <c r="AG34" s="23"/>
       <c r="AH34" s="23"/>
     </row>
-    <row r="35" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:34">
       <c r="C35" t="s">
         <v>47</v>
       </c>
@@ -3811,7 +3906,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:34">
       <c r="C36" t="s">
         <v>48</v>
       </c>
@@ -3825,7 +3920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:34">
       <c r="C37" t="s">
         <v>49</v>
       </c>
@@ -3839,7 +3934,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:34">
       <c r="C38" t="s">
         <v>50</v>
       </c>
@@ -3867,7 +3962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:34">
       <c r="C39" t="s">
         <v>31</v>
       </c>
@@ -3895,7 +3990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:34">
       <c r="C40" t="s">
         <v>26</v>
       </c>
@@ -3911,7 +4006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:34">
       <c r="G41">
         <v>11</v>
       </c>
@@ -3920,13 +4015,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:34">
       <c r="G42">
         <f>SUM(G38:G41)</f>
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:34">
       <c r="H44">
         <v>9</v>
       </c>
@@ -3935,7 +4030,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:34">
       <c r="H45">
         <f>H44-2</f>
         <v>7</v>
@@ -3945,7 +4040,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:34">
       <c r="H46">
         <f t="shared" ref="H46:H48" si="24">H45-2</f>
         <v>5</v>
@@ -3955,7 +4050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:34">
       <c r="H47">
         <f t="shared" si="24"/>
         <v>3</v>
@@ -3965,7 +4060,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:34">
       <c r="H48">
         <f t="shared" si="24"/>
         <v>1</v>
@@ -3975,7 +4070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="8:14">
       <c r="H49">
         <f>SUM(H44:H48)</f>
         <v>25</v>
@@ -3987,7 +4082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="8:14">
       <c r="L50" t="s">
         <v>84</v>
       </c>
@@ -4025,11 +4120,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V40"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
@@ -4047,8 +4142,8 @@
     <col min="19" max="38" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:22" ht="60">
       <c r="G3" s="1" t="s">
         <v>74</v>
       </c>
@@ -4090,7 +4185,7 @@
       </c>
       <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="30" customHeight="1">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -4153,7 +4248,7 @@
         <v>SC:1[ MATH101] [Electronics][John][ComLab 1] RQ: 1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="30" customHeight="1">
       <c r="A5">
         <v>1</v>
       </c>
@@ -4218,7 +4313,7 @@
 ][Room 2] RQ: 1</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="30" customHeight="1">
       <c r="A6">
         <v>2</v>
       </c>
@@ -4281,7 +4376,7 @@
         <v>SC:3[ ENGL101] [Electronics][James][Room 1] RQ: 3</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="30" customHeight="1">
       <c r="A7">
         <v>3</v>
       </c>
@@ -4344,7 +4439,7 @@
         <v>SC:4[ MATH101] [Mechtronics][John][ComLab 1] RQ: 1</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="30" customHeight="1">
       <c r="A8">
         <v>4</v>
       </c>
@@ -4409,7 +4504,7 @@
 ][Room 1] RQ: 1</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" ht="30" customHeight="1" thickBot="1">
       <c r="G9" s="1">
         <v>6</v>
       </c>
@@ -4460,7 +4555,7 @@
         <v>SC:6[ ENGL101] [Mechtronics][James][Room 1] RQ: 3</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -4477,7 +4572,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22">
       <c r="A13">
         <v>1</v>
       </c>
@@ -4494,7 +4589,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22">
       <c r="A14">
         <v>2</v>
       </c>
@@ -4521,7 +4616,7 @@
       </c>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22">
       <c r="A15">
         <v>3</v>
       </c>
@@ -4548,7 +4643,7 @@
       </c>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22">
       <c r="G16" s="2">
         <v>13</v>
       </c>
@@ -4560,7 +4655,7 @@
       </c>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="G17" s="96">
         <v>2</v>
       </c>
@@ -4572,7 +4667,7 @@
       </c>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="G18" s="96">
         <v>5</v>
       </c>
@@ -4584,7 +4679,7 @@
       </c>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -4611,7 +4706,7 @@
       </c>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>1</v>
       </c>
@@ -4638,7 +4733,7 @@
       </c>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>2</v>
       </c>
@@ -4665,7 +4760,7 @@
       </c>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="G22" s="2">
         <v>10</v>
       </c>
@@ -4677,7 +4772,7 @@
       </c>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="G23" s="2">
         <v>11</v>
       </c>
@@ -4689,7 +4784,7 @@
       </c>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="G24" s="2">
         <v>12</v>
       </c>
@@ -4701,7 +4796,7 @@
       </c>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -4728,7 +4823,7 @@
       </c>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>1</v>
       </c>
@@ -4755,7 +4850,7 @@
       </c>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>2</v>
       </c>
@@ -4782,7 +4877,7 @@
       </c>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>3</v>
       </c>
@@ -4809,7 +4904,7 @@
       </c>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>4</v>
       </c>
@@ -4836,7 +4931,7 @@
       </c>
       <c r="J29" s="95"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="G30" s="96">
         <v>8</v>
       </c>
@@ -4848,42 +4943,42 @@
       </c>
       <c r="J30" s="95"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3">
       <c r="C33" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3">
       <c r="C34" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3">
       <c r="C35" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3">
       <c r="C36" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3">
       <c r="C37" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3">
       <c r="C38" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3">
       <c r="C39" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:3">
       <c r="C40" t="s">
         <v>26</v>
       </c>
@@ -4928,21 +5023,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:W29"/>
+  <dimension ref="C1:AB123"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView showGridLines="0" topLeftCell="E86" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J123" sqref="J123:M123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="9" width="10.7109375" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" customWidth="1"/>
-    <col min="11" max="19" width="10.7109375" customWidth="1"/>
+    <col min="11" max="17" width="10.7109375" customWidth="1"/>
+    <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" customWidth="1"/>
     <col min="20" max="20" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:23" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:23" ht="17.25">
       <c r="C1" s="104" t="s">
         <v>85</v>
       </c>
@@ -4950,21 +5047,21 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:23">
       <c r="M2" s="103"/>
     </row>
-    <row r="3" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:23">
       <c r="M3" s="105">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:23">
       <c r="C4">
         <v>0</v>
       </c>
       <c r="M4" s="103"/>
     </row>
-    <row r="5" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:23">
       <c r="C5" s="1" t="s">
         <v>86</v>
       </c>
@@ -5008,7 +5105,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:23">
       <c r="C6" s="1" t="s">
         <v>92</v>
       </c>
@@ -5052,7 +5149,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:23" ht="15.75" thickBot="1">
       <c r="C7" s="1" t="s">
         <v>98</v>
       </c>
@@ -5096,7 +5193,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:23" ht="18.75">
       <c r="C8" s="2">
         <v>12</v>
       </c>
@@ -5148,7 +5245,7 @@
       <c r="U8" s="95"/>
       <c r="W8" s="95"/>
     </row>
-    <row r="9" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:23" ht="18.75">
       <c r="C9" s="97">
         <v>13</v>
       </c>
@@ -5200,7 +5297,7 @@
       <c r="U9" s="95"/>
       <c r="W9" s="95"/>
     </row>
-    <row r="10" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:23" ht="18.75">
       <c r="C10" s="97">
         <v>18</v>
       </c>
@@ -5252,7 +5349,7 @@
       <c r="U10" s="95"/>
       <c r="W10" s="95"/>
     </row>
-    <row r="11" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:23" ht="18.75">
       <c r="C11" s="96">
         <v>6</v>
       </c>
@@ -5304,7 +5401,7 @@
       <c r="U11" s="95"/>
       <c r="W11" s="95"/>
     </row>
-    <row r="12" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:23" ht="18.75">
       <c r="C12" s="96">
         <v>21</v>
       </c>
@@ -5356,7 +5453,7 @@
       <c r="U12" s="95"/>
       <c r="W12" s="95"/>
     </row>
-    <row r="13" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:23" ht="18.75">
       <c r="C13" s="98">
         <v>2</v>
       </c>
@@ -5408,7 +5505,7 @@
       <c r="U13" s="95"/>
       <c r="W13" s="95"/>
     </row>
-    <row r="14" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:23" ht="18.75">
       <c r="C14" s="98">
         <v>8</v>
       </c>
@@ -5460,7 +5557,7 @@
       <c r="U14" s="95"/>
       <c r="W14" s="95"/>
     </row>
-    <row r="15" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:23" ht="18.75">
       <c r="C15" s="99">
         <v>9</v>
       </c>
@@ -5512,7 +5609,7 @@
       <c r="U15" s="95"/>
       <c r="W15" s="95"/>
     </row>
-    <row r="16" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:23" ht="18.75">
       <c r="C16" s="99">
         <v>3</v>
       </c>
@@ -5564,7 +5661,7 @@
       <c r="U16" s="95"/>
       <c r="W16" s="95"/>
     </row>
-    <row r="17" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:23" ht="18.75">
       <c r="C17" s="100">
         <v>15</v>
       </c>
@@ -5616,7 +5713,7 @@
       <c r="U17" s="95"/>
       <c r="W17" s="95"/>
     </row>
-    <row r="18" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:23" ht="18.75">
       <c r="C18" s="100">
         <v>16</v>
       </c>
@@ -5668,7 +5765,7 @@
       <c r="U18" s="95"/>
       <c r="W18" s="95"/>
     </row>
-    <row r="19" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:23" ht="18.75">
       <c r="C19" s="101">
         <v>4</v>
       </c>
@@ -5720,7 +5817,7 @@
       <c r="U19" s="95"/>
       <c r="W19" s="95"/>
     </row>
-    <row r="20" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:23" ht="18.75">
       <c r="C20" s="101">
         <v>20</v>
       </c>
@@ -5772,7 +5869,7 @@
       <c r="U20" s="95"/>
       <c r="W20" s="95"/>
     </row>
-    <row r="21" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:23" ht="18.75">
       <c r="C21" s="2">
         <v>5</v>
       </c>
@@ -5824,7 +5921,7 @@
       <c r="U21" s="95"/>
       <c r="W21" s="95"/>
     </row>
-    <row r="22" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:23" ht="18.75">
       <c r="C22" s="2">
         <v>10</v>
       </c>
@@ -5876,7 +5973,7 @@
       <c r="U22" s="95"/>
       <c r="W22" s="95"/>
     </row>
-    <row r="23" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:23" ht="18.75">
       <c r="C23" s="97">
         <v>17</v>
       </c>
@@ -5928,7 +6025,7 @@
       <c r="U23" s="95"/>
       <c r="W23" s="95"/>
     </row>
-    <row r="24" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:23" ht="18.75">
       <c r="C24" s="97">
         <v>11</v>
       </c>
@@ -5980,7 +6077,7 @@
       <c r="U24" s="95"/>
       <c r="W24" s="95"/>
     </row>
-    <row r="25" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:23" ht="18.75">
       <c r="C25" s="2">
         <v>7</v>
       </c>
@@ -6032,7 +6129,7 @@
       <c r="U25" s="95"/>
       <c r="W25" s="95"/>
     </row>
-    <row r="26" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:23" ht="18.75">
       <c r="C26" s="96">
         <v>19</v>
       </c>
@@ -6084,7 +6181,7 @@
       <c r="U26" s="95"/>
       <c r="W26" s="95"/>
     </row>
-    <row r="27" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:23" ht="18.75">
       <c r="C27" s="96">
         <v>0</v>
       </c>
@@ -6136,7 +6233,7 @@
       <c r="U27" s="95"/>
       <c r="W27" s="95"/>
     </row>
-    <row r="28" spans="3:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:23" ht="18.75">
       <c r="C28" s="102">
         <v>1</v>
       </c>
@@ -6188,7 +6285,7 @@
       <c r="U28" s="95"/>
       <c r="W28" s="95"/>
     </row>
-    <row r="29" spans="3:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:23" ht="19.5" thickBot="1">
       <c r="C29" s="102">
         <v>14</v>
       </c>
@@ -6240,8 +6337,1530 @@
       <c r="U29" s="95"/>
       <c r="W29" s="95"/>
     </row>
+    <row r="50" spans="3:24" ht="15.75" thickBot="1">
+      <c r="C50" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="3:24" ht="18.75">
+      <c r="C51" s="141"/>
+      <c r="D51" s="141"/>
+      <c r="E51" s="142"/>
+      <c r="F51" s="141"/>
+      <c r="G51" s="141"/>
+      <c r="H51" s="141"/>
+      <c r="I51" s="141"/>
+      <c r="J51" s="141"/>
+      <c r="W51">
+        <v>3</v>
+      </c>
+      <c r="X51" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="3:24" ht="18.75">
+      <c r="C52" s="141"/>
+      <c r="D52" s="141"/>
+      <c r="E52" s="143"/>
+      <c r="F52" s="141"/>
+      <c r="G52" s="141"/>
+      <c r="H52" s="141"/>
+      <c r="I52" s="141"/>
+      <c r="J52" s="141"/>
+      <c r="W52">
+        <v>3</v>
+      </c>
+      <c r="X52" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="3:24" ht="18.75">
+      <c r="C53" s="141"/>
+      <c r="D53" s="141"/>
+      <c r="E53" s="143"/>
+      <c r="F53" s="141"/>
+      <c r="G53" s="141"/>
+      <c r="H53" s="141"/>
+      <c r="I53" s="141"/>
+      <c r="J53" s="141"/>
+      <c r="W53">
+        <v>4</v>
+      </c>
+      <c r="X53" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="3:24" ht="18.75">
+      <c r="C54" s="141"/>
+      <c r="D54" s="141"/>
+      <c r="E54" s="143"/>
+      <c r="F54" s="141"/>
+      <c r="G54" s="141"/>
+      <c r="H54" s="141"/>
+      <c r="I54" s="141"/>
+      <c r="J54" s="141"/>
+      <c r="W54">
+        <v>3</v>
+      </c>
+      <c r="X54" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="3:24" ht="18.75">
+      <c r="C55" s="141"/>
+      <c r="D55" s="141"/>
+      <c r="E55" s="143"/>
+      <c r="F55" s="141"/>
+      <c r="G55" s="141"/>
+      <c r="H55" s="141"/>
+      <c r="I55" s="141"/>
+      <c r="J55" s="141"/>
+      <c r="W55">
+        <v>4</v>
+      </c>
+      <c r="X55" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="3:24" ht="18.75">
+      <c r="C56" s="141"/>
+      <c r="D56" s="141"/>
+      <c r="E56" s="143"/>
+      <c r="F56" s="141"/>
+      <c r="G56" s="141"/>
+      <c r="H56" s="141"/>
+      <c r="I56" s="141"/>
+      <c r="J56" s="141"/>
+      <c r="W56">
+        <v>2</v>
+      </c>
+      <c r="X56" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="3:24" ht="18.75">
+      <c r="C57" s="141"/>
+      <c r="D57" s="141"/>
+      <c r="E57" s="143"/>
+      <c r="F57" s="141"/>
+      <c r="G57" s="141"/>
+      <c r="H57" s="141"/>
+      <c r="I57" s="141"/>
+      <c r="J57" s="141"/>
+      <c r="W57">
+        <v>1</v>
+      </c>
+      <c r="X57" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="3:24" ht="18.75">
+      <c r="C58" s="141"/>
+      <c r="D58" s="141"/>
+      <c r="E58" s="143"/>
+      <c r="F58" s="141"/>
+      <c r="G58" s="141"/>
+      <c r="H58" s="141"/>
+      <c r="I58" s="141"/>
+      <c r="J58" s="141"/>
+      <c r="W58">
+        <v>1</v>
+      </c>
+      <c r="X58" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="3:24" ht="18.75">
+      <c r="C59" s="141"/>
+      <c r="D59" s="141"/>
+      <c r="E59" s="143"/>
+      <c r="F59" s="141"/>
+      <c r="G59" s="141"/>
+      <c r="H59" s="141"/>
+      <c r="I59" s="141"/>
+      <c r="J59" s="141"/>
+      <c r="W59">
+        <v>2</v>
+      </c>
+      <c r="X59" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="3:24" ht="18.75">
+      <c r="C60" s="141"/>
+      <c r="D60" s="141"/>
+      <c r="E60" s="143"/>
+      <c r="F60" s="141"/>
+      <c r="G60" s="141"/>
+      <c r="H60" s="141"/>
+      <c r="I60" s="141"/>
+      <c r="J60" s="141"/>
+      <c r="W60">
+        <v>3</v>
+      </c>
+      <c r="X60" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="3:24" ht="18.75">
+      <c r="C61" s="141"/>
+      <c r="D61" s="141"/>
+      <c r="E61" s="143"/>
+      <c r="F61" s="141"/>
+      <c r="G61" s="141"/>
+      <c r="H61" s="141"/>
+      <c r="I61" s="141"/>
+      <c r="J61" s="141"/>
+      <c r="W61">
+        <v>4</v>
+      </c>
+      <c r="X61" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="3:24" ht="18.75">
+      <c r="C62" s="141"/>
+      <c r="D62" s="141"/>
+      <c r="E62" s="143"/>
+      <c r="F62" s="141"/>
+      <c r="G62" s="141"/>
+      <c r="H62" s="141"/>
+      <c r="I62" s="141"/>
+      <c r="J62" s="141"/>
+      <c r="T62" t="s">
+        <v>176</v>
+      </c>
+      <c r="V62" t="s">
+        <v>176</v>
+      </c>
+      <c r="W62">
+        <v>3</v>
+      </c>
+      <c r="X62" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="3:24" ht="18.75">
+      <c r="C63" s="141"/>
+      <c r="D63" s="141"/>
+      <c r="E63" s="143"/>
+      <c r="F63" s="141"/>
+      <c r="G63" s="141"/>
+      <c r="H63" s="141"/>
+      <c r="I63" s="141"/>
+      <c r="J63" s="141"/>
+      <c r="V63" t="s">
+        <v>176</v>
+      </c>
+      <c r="W63">
+        <v>4</v>
+      </c>
+      <c r="X63" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="64" spans="3:24" ht="18.75">
+      <c r="C64" s="141"/>
+      <c r="D64" s="141"/>
+      <c r="E64" s="143"/>
+      <c r="F64" s="141"/>
+      <c r="G64" s="141"/>
+      <c r="H64" s="141"/>
+      <c r="I64" s="141"/>
+      <c r="J64" s="141"/>
+      <c r="T64" t="s">
+        <v>176</v>
+      </c>
+      <c r="W64">
+        <v>3</v>
+      </c>
+      <c r="X64" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="3:28" ht="18.75">
+      <c r="C65" s="141"/>
+      <c r="D65" s="141"/>
+      <c r="E65" s="143"/>
+      <c r="F65" s="141"/>
+      <c r="G65" s="141"/>
+      <c r="H65" s="141"/>
+      <c r="I65" s="141"/>
+      <c r="J65" s="141"/>
+      <c r="W65">
+        <v>2</v>
+      </c>
+      <c r="X65" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="3:28" ht="18.75">
+      <c r="C66" s="141"/>
+      <c r="D66" s="141"/>
+      <c r="E66" s="143"/>
+      <c r="F66" s="141"/>
+      <c r="G66" s="141"/>
+      <c r="H66" s="141"/>
+      <c r="I66" s="141"/>
+      <c r="J66" s="141"/>
+      <c r="W66">
+        <v>4</v>
+      </c>
+      <c r="X66" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="67" spans="3:28" ht="18.75">
+      <c r="C67" s="141"/>
+      <c r="D67" s="141"/>
+      <c r="E67" s="143"/>
+      <c r="F67" s="141"/>
+      <c r="G67" s="141"/>
+      <c r="H67" s="141"/>
+      <c r="I67" s="141"/>
+      <c r="J67" s="141"/>
+      <c r="W67">
+        <v>2</v>
+      </c>
+      <c r="X67" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="3:28" ht="18.75">
+      <c r="C68" s="141"/>
+      <c r="D68" s="141"/>
+      <c r="E68" s="143"/>
+      <c r="F68" s="141"/>
+      <c r="G68" s="141"/>
+      <c r="H68" s="141"/>
+      <c r="I68" s="141"/>
+      <c r="J68" s="141"/>
+      <c r="W68">
+        <v>3</v>
+      </c>
+      <c r="X68" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="3:28" ht="18.75">
+      <c r="C69" s="141"/>
+      <c r="D69" s="141"/>
+      <c r="E69" s="143"/>
+      <c r="F69" s="141"/>
+      <c r="G69" s="141"/>
+      <c r="H69" s="141"/>
+      <c r="I69" s="141"/>
+      <c r="J69" s="141"/>
+      <c r="W69">
+        <v>4</v>
+      </c>
+      <c r="X69" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="70" spans="3:28" ht="18.75">
+      <c r="C70" s="141"/>
+      <c r="D70" s="141"/>
+      <c r="E70" s="143"/>
+      <c r="F70" s="141"/>
+      <c r="G70" s="141"/>
+      <c r="H70" s="141"/>
+      <c r="I70" s="141"/>
+      <c r="J70" s="141"/>
+      <c r="W70">
+        <v>1</v>
+      </c>
+      <c r="X70" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="3:28" ht="18.75">
+      <c r="C71" s="141"/>
+      <c r="D71" s="141"/>
+      <c r="E71" s="143"/>
+      <c r="F71" s="141"/>
+      <c r="G71" s="141"/>
+      <c r="H71" s="141"/>
+      <c r="I71" s="141"/>
+      <c r="J71" s="141"/>
+      <c r="V71" t="s">
+        <v>176</v>
+      </c>
+      <c r="W71">
+        <v>1</v>
+      </c>
+      <c r="X71" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="3:28" ht="19.5" thickBot="1">
+      <c r="C72" s="141"/>
+      <c r="D72" s="141"/>
+      <c r="E72" s="144"/>
+      <c r="F72" s="141"/>
+      <c r="G72" s="141"/>
+      <c r="H72" s="141"/>
+      <c r="I72" s="141"/>
+      <c r="J72" s="141"/>
+      <c r="V72" t="s">
+        <v>176</v>
+      </c>
+      <c r="W72">
+        <v>3</v>
+      </c>
+      <c r="X72" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="3:28" ht="15.75" thickBot="1"/>
+    <row r="80" spans="3:28">
+      <c r="I80" s="149" t="s">
+        <v>25</v>
+      </c>
+      <c r="J80" s="150"/>
+      <c r="K80" s="150"/>
+      <c r="L80" s="150"/>
+      <c r="M80" s="151"/>
+      <c r="N80" s="152" t="s">
+        <v>178</v>
+      </c>
+      <c r="O80" s="153"/>
+      <c r="P80" s="153"/>
+      <c r="Q80" s="153"/>
+      <c r="R80" s="154"/>
+      <c r="S80" s="149" t="s">
+        <v>70</v>
+      </c>
+      <c r="T80" s="150"/>
+      <c r="U80" s="150"/>
+      <c r="V80" s="150"/>
+      <c r="W80" s="151"/>
+      <c r="X80" s="152" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y80" s="153"/>
+      <c r="Z80" s="153"/>
+      <c r="AA80" s="153"/>
+      <c r="AB80" s="154"/>
+    </row>
+    <row r="81" spans="4:28" ht="15.75" thickBot="1">
+      <c r="D81" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J81" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="K81" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="L81" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="M81" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="N81" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="O81" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="P81" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q81" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="R81" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="S81" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="T81" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="U81" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="V81" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="W81" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="X81" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y81" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z81" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA81" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB81" s="39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="82" spans="4:28">
+      <c r="D82" s="3">
+        <v>1</v>
+      </c>
+      <c r="E82" s="3">
+        <v>1</v>
+      </c>
+      <c r="F82" s="3">
+        <v>0</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H82" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I82" s="52"/>
+      <c r="J82" s="64"/>
+      <c r="K82" s="54"/>
+      <c r="L82" s="53"/>
+      <c r="M82" s="55"/>
+      <c r="N82" s="2">
+        <v>6</v>
+      </c>
+      <c r="O82" s="2" t="str">
+        <f>CONCATENATE(W51,X51)</f>
+        <v>3ENGL101</v>
+      </c>
+      <c r="P82" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q82" s="2">
+        <v>3</v>
+      </c>
+      <c r="R82" s="43"/>
+      <c r="S82" s="33"/>
+      <c r="T82" s="72"/>
+      <c r="U82" s="35"/>
+      <c r="V82" s="34"/>
+      <c r="W82" s="36"/>
+      <c r="X82" s="40"/>
+      <c r="Y82" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z82" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA82" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="AB82" s="43" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="83" spans="4:28">
+      <c r="D83" s="3">
+        <v>1</v>
+      </c>
+      <c r="E83" s="3">
+        <v>2</v>
+      </c>
+      <c r="F83" s="3">
+        <v>1</v>
+      </c>
+      <c r="G83" s="3"/>
+      <c r="H83" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I83" s="11"/>
+      <c r="J83" s="12"/>
+      <c r="K83" s="13"/>
+      <c r="L83" s="12"/>
+      <c r="M83" s="14"/>
+      <c r="N83" s="2">
+        <v>6</v>
+      </c>
+      <c r="O83" s="2" t="str">
+        <f>CONCATENATE(W52,X52)</f>
+        <v>3ENGL101</v>
+      </c>
+      <c r="P83" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q83" s="2">
+        <v>3</v>
+      </c>
+      <c r="R83" s="47"/>
+      <c r="S83" s="25"/>
+      <c r="T83" s="73"/>
+      <c r="U83" s="27"/>
+      <c r="V83" s="26"/>
+      <c r="W83" s="28"/>
+      <c r="X83" s="2">
+        <v>7</v>
+      </c>
+      <c r="Y83" s="2" t="str">
+        <f>CONCATENATE(W53,X53)</f>
+        <v>4Study Break</v>
+      </c>
+      <c r="Z83" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA83" s="2">
+        <v>5</v>
+      </c>
+      <c r="AB83" s="47" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="84" spans="4:28">
+      <c r="D84" s="3">
+        <v>1</v>
+      </c>
+      <c r="E84" s="3">
+        <v>3</v>
+      </c>
+      <c r="F84" s="3">
+        <v>2</v>
+      </c>
+      <c r="G84" s="3"/>
+      <c r="H84" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I84" s="25"/>
+      <c r="J84" s="65"/>
+      <c r="K84" s="27"/>
+      <c r="L84" s="26"/>
+      <c r="M84" s="28"/>
+      <c r="N84" s="2">
+        <v>3</v>
+      </c>
+      <c r="O84" s="2" t="str">
+        <f>CONCATENATE(W54,X54)</f>
+        <v>3ENGL101</v>
+      </c>
+      <c r="P84" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q84" s="2">
+        <v>3</v>
+      </c>
+      <c r="R84" s="47"/>
+      <c r="S84" s="11"/>
+      <c r="T84" s="12"/>
+      <c r="U84" s="13"/>
+      <c r="V84" s="12"/>
+      <c r="W84" s="14"/>
+      <c r="X84" s="2">
+        <v>8</v>
+      </c>
+      <c r="Y84" s="2" t="str">
+        <f>CONCATENATE(W55,X55)</f>
+        <v>4Study Break</v>
+      </c>
+      <c r="Z84" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA84" s="2">
+        <v>5</v>
+      </c>
+      <c r="AB84" s="47" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="85" spans="4:28">
+      <c r="D85" s="3">
+        <v>1</v>
+      </c>
+      <c r="E85" s="3">
+        <v>4</v>
+      </c>
+      <c r="F85" s="3">
+        <v>3</v>
+      </c>
+      <c r="G85" s="3"/>
+      <c r="H85" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I85" s="25"/>
+      <c r="J85" s="70"/>
+      <c r="K85" s="27"/>
+      <c r="L85" s="26"/>
+      <c r="M85" s="28"/>
+      <c r="N85" s="44"/>
+      <c r="O85" s="45"/>
+      <c r="P85" s="46"/>
+      <c r="Q85" s="45"/>
+      <c r="R85" s="47"/>
+      <c r="S85" s="56"/>
+      <c r="T85" s="74"/>
+      <c r="U85" s="58"/>
+      <c r="V85" s="57"/>
+      <c r="W85" s="59"/>
+      <c r="X85" s="44"/>
+      <c r="Y85" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z85" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA85" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="AB85" s="47" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="86" spans="4:28" ht="15.75" thickBot="1">
+      <c r="D86" s="3">
+        <v>1</v>
+      </c>
+      <c r="E86" s="3">
+        <v>5</v>
+      </c>
+      <c r="F86" s="3">
+        <v>4</v>
+      </c>
+      <c r="G86" s="3"/>
+      <c r="H86" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I86" s="29"/>
+      <c r="J86" s="71"/>
+      <c r="K86" s="31"/>
+      <c r="L86" s="30"/>
+      <c r="M86" s="32"/>
+      <c r="N86" s="48"/>
+      <c r="O86" s="49"/>
+      <c r="P86" s="50"/>
+      <c r="Q86" s="49"/>
+      <c r="R86" s="51"/>
+      <c r="S86" s="60"/>
+      <c r="T86" s="75"/>
+      <c r="U86" s="62"/>
+      <c r="V86" s="61"/>
+      <c r="W86" s="63"/>
+      <c r="X86" s="48"/>
+      <c r="Y86" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z86" s="50" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA86" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="AB86" s="51" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="87" spans="4:28">
+      <c r="D87" s="77">
+        <v>2</v>
+      </c>
+      <c r="E87" s="77">
+        <v>1</v>
+      </c>
+      <c r="F87" s="77">
+        <v>5</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H87" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I87" s="52"/>
+      <c r="J87" s="68"/>
+      <c r="K87" s="54"/>
+      <c r="L87" s="53"/>
+      <c r="M87" s="55"/>
+      <c r="N87" s="2">
+        <v>2</v>
+      </c>
+      <c r="O87" s="2" t="str">
+        <f>CONCATENATE(W56,X56)</f>
+        <v>2POLSC101</v>
+      </c>
+      <c r="P87" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q87" s="2">
+        <v>1</v>
+      </c>
+      <c r="R87" s="43"/>
+      <c r="S87" s="2">
+        <v>4</v>
+      </c>
+      <c r="T87" s="2" t="str">
+        <f>CONCATENATE(W57,X57)</f>
+        <v>1MATH101</v>
+      </c>
+      <c r="U87" s="2">
+        <v>2</v>
+      </c>
+      <c r="V87" s="2">
+        <v>4</v>
+      </c>
+      <c r="W87" s="22"/>
+      <c r="X87" s="40"/>
+      <c r="Y87" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z87" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA87" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="AB87" s="43" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="88" spans="4:28">
+      <c r="D88" s="77">
+        <v>2</v>
+      </c>
+      <c r="E88" s="77">
+        <v>2</v>
+      </c>
+      <c r="F88" s="77">
+        <v>6</v>
+      </c>
+      <c r="G88" s="3"/>
+      <c r="H88" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I88" s="56"/>
+      <c r="J88" s="69"/>
+      <c r="K88" s="58"/>
+      <c r="L88" s="57"/>
+      <c r="M88" s="59"/>
+      <c r="N88" s="2">
+        <v>2</v>
+      </c>
+      <c r="O88" s="2" t="str">
+        <f>CONCATENATE(W59,X59)</f>
+        <v>2POLSC101</v>
+      </c>
+      <c r="P88" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q88" s="2">
+        <v>1</v>
+      </c>
+      <c r="R88" s="47"/>
+      <c r="S88" s="2">
+        <v>4</v>
+      </c>
+      <c r="T88" s="2" t="str">
+        <f>CONCATENATE(W58,X58)</f>
+        <v>1MATH101</v>
+      </c>
+      <c r="U88" s="2">
+        <v>2</v>
+      </c>
+      <c r="V88" s="2">
+        <v>4</v>
+      </c>
+      <c r="W88" s="14"/>
+      <c r="X88" s="44"/>
+      <c r="Y88" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z88" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA88" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="AB88" s="47" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="89" spans="4:28">
+      <c r="D89" s="77">
+        <v>2</v>
+      </c>
+      <c r="E89" s="77">
+        <v>3</v>
+      </c>
+      <c r="F89" s="77">
+        <v>7</v>
+      </c>
+      <c r="G89" s="3"/>
+      <c r="H89" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I89" s="56"/>
+      <c r="J89" s="66"/>
+      <c r="K89" s="58"/>
+      <c r="L89" s="57"/>
+      <c r="M89" s="59"/>
+      <c r="N89" s="2">
+        <v>6</v>
+      </c>
+      <c r="O89" s="2" t="str">
+        <f>CONCATENATE(W60,X60)</f>
+        <v>3ENGL101</v>
+      </c>
+      <c r="P89" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q89" s="2">
+        <v>3</v>
+      </c>
+      <c r="R89" s="47"/>
+      <c r="S89" s="11"/>
+      <c r="T89" s="12"/>
+      <c r="U89" s="13"/>
+      <c r="V89" s="12"/>
+      <c r="W89" s="14"/>
+      <c r="X89" s="2">
+        <v>7</v>
+      </c>
+      <c r="Y89" s="2" t="str">
+        <f>CONCATENATE(W61,X61)</f>
+        <v>4Study Break</v>
+      </c>
+      <c r="Z89" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA89" s="2">
+        <v>5</v>
+      </c>
+      <c r="AB89" s="47" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="90" spans="4:28">
+      <c r="D90" s="77">
+        <v>2</v>
+      </c>
+      <c r="E90" s="77">
+        <v>4</v>
+      </c>
+      <c r="F90" s="77">
+        <v>8</v>
+      </c>
+      <c r="G90" s="3"/>
+      <c r="H90" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I90" s="25"/>
+      <c r="J90" s="65"/>
+      <c r="K90" s="27"/>
+      <c r="L90" s="26"/>
+      <c r="M90" s="28"/>
+      <c r="N90" s="2">
+        <v>3</v>
+      </c>
+      <c r="O90" s="2" t="str">
+        <f>CONCATENATE(W62,X62)</f>
+        <v>3ENGL101</v>
+      </c>
+      <c r="P90" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q90" s="2">
+        <v>3</v>
+      </c>
+      <c r="R90" s="47"/>
+      <c r="S90" s="11"/>
+      <c r="T90" s="12"/>
+      <c r="U90" s="13"/>
+      <c r="V90" s="12"/>
+      <c r="W90" s="14"/>
+      <c r="X90" s="2">
+        <v>8</v>
+      </c>
+      <c r="Y90" s="2" t="str">
+        <f>CONCATENATE(W63,X63)</f>
+        <v>4Study Break</v>
+      </c>
+      <c r="Z90" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA90" s="2">
+        <v>5</v>
+      </c>
+      <c r="AB90" s="47" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="91" spans="4:28" ht="15.75" thickBot="1">
+      <c r="D91" s="77">
+        <v>2</v>
+      </c>
+      <c r="E91" s="77">
+        <v>5</v>
+      </c>
+      <c r="F91" s="77">
+        <v>9</v>
+      </c>
+      <c r="G91" s="3"/>
+      <c r="H91" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I91" s="29"/>
+      <c r="J91" s="67"/>
+      <c r="K91" s="31"/>
+      <c r="L91" s="30"/>
+      <c r="M91" s="32"/>
+      <c r="N91" s="2">
+        <v>3</v>
+      </c>
+      <c r="O91" s="2" t="str">
+        <f>CONCATENATE(W64,X64)</f>
+        <v>3ENGL101</v>
+      </c>
+      <c r="P91" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q91" s="2">
+        <v>3</v>
+      </c>
+      <c r="R91" s="51"/>
+      <c r="S91" s="15"/>
+      <c r="T91" s="16"/>
+      <c r="U91" s="17"/>
+      <c r="V91" s="16"/>
+      <c r="W91" s="18"/>
+      <c r="X91" s="48"/>
+      <c r="Y91" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z91" s="50" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA91" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="AB91" s="51" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="92" spans="4:28">
+      <c r="D92" s="3">
+        <v>3</v>
+      </c>
+      <c r="E92" s="3">
+        <v>1</v>
+      </c>
+      <c r="F92" s="3">
+        <v>10</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H92" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I92" s="52"/>
+      <c r="J92" s="64"/>
+      <c r="K92" s="54"/>
+      <c r="L92" s="53"/>
+      <c r="M92" s="55"/>
+      <c r="N92" s="19">
+        <v>5</v>
+      </c>
+      <c r="O92" s="20" t="str">
+        <f>CONCATENATE(W65,X65)</f>
+        <v>2POLSC101</v>
+      </c>
+      <c r="P92" s="21">
+        <v>2</v>
+      </c>
+      <c r="Q92" s="20">
+        <v>1</v>
+      </c>
+      <c r="R92" s="43"/>
+      <c r="S92" s="19"/>
+      <c r="T92" s="20"/>
+      <c r="U92" s="21"/>
+      <c r="V92" s="20"/>
+      <c r="W92" s="22"/>
+      <c r="X92" s="40"/>
+      <c r="Y92" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z92" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA92" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="AB92" s="43" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="93" spans="4:28">
+      <c r="D93" s="3">
+        <v>3</v>
+      </c>
+      <c r="E93" s="3">
+        <v>2</v>
+      </c>
+      <c r="F93" s="3">
+        <v>11</v>
+      </c>
+      <c r="G93" s="3"/>
+      <c r="H93" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I93" s="56"/>
+      <c r="J93" s="66"/>
+      <c r="K93" s="58"/>
+      <c r="L93" s="57"/>
+      <c r="M93" s="59"/>
+      <c r="N93" s="2">
+        <v>5</v>
+      </c>
+      <c r="O93" s="2" t="str">
+        <f>CONCATENATE(W67,X67)</f>
+        <v>2POLSC101</v>
+      </c>
+      <c r="P93" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q93" s="2">
+        <v>1</v>
+      </c>
+      <c r="R93" s="47"/>
+      <c r="S93" s="11"/>
+      <c r="T93" s="12"/>
+      <c r="U93" s="13"/>
+      <c r="V93" s="12"/>
+      <c r="W93" s="14"/>
+      <c r="X93" s="2">
+        <v>7</v>
+      </c>
+      <c r="Y93" s="2" t="str">
+        <f>CONCATENATE(W66,X66)</f>
+        <v>4Study Break</v>
+      </c>
+      <c r="Z93" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA93" s="2">
+        <v>5</v>
+      </c>
+      <c r="AB93" s="47" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="94" spans="4:28">
+      <c r="D94" s="3">
+        <v>3</v>
+      </c>
+      <c r="E94" s="3">
+        <v>3</v>
+      </c>
+      <c r="F94" s="3">
+        <v>12</v>
+      </c>
+      <c r="G94" s="3"/>
+      <c r="H94" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I94" s="25"/>
+      <c r="J94" s="65"/>
+      <c r="K94" s="27"/>
+      <c r="L94" s="26"/>
+      <c r="M94" s="28"/>
+      <c r="N94" s="2">
+        <v>3</v>
+      </c>
+      <c r="O94" s="2" t="str">
+        <f>CONCATENATE(W68,X68)</f>
+        <v>3ENGL101</v>
+      </c>
+      <c r="P94" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q94" s="2">
+        <v>3</v>
+      </c>
+      <c r="R94" s="47"/>
+      <c r="S94" s="11"/>
+      <c r="T94" s="12"/>
+      <c r="U94" s="13"/>
+      <c r="V94" s="12"/>
+      <c r="W94" s="14"/>
+      <c r="X94" s="44"/>
+      <c r="Y94" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z94" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA94" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="AB94" s="47" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="95" spans="4:28">
+      <c r="D95" s="3">
+        <v>3</v>
+      </c>
+      <c r="E95" s="3">
+        <v>4</v>
+      </c>
+      <c r="F95" s="3">
+        <v>13</v>
+      </c>
+      <c r="G95" s="3"/>
+      <c r="H95" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I95" s="11"/>
+      <c r="J95" s="12"/>
+      <c r="K95" s="13"/>
+      <c r="L95" s="12"/>
+      <c r="M95" s="14"/>
+      <c r="N95" s="44"/>
+      <c r="O95" s="45"/>
+      <c r="P95" s="46"/>
+      <c r="Q95" s="45"/>
+      <c r="R95" s="47"/>
+      <c r="S95" s="2">
+        <v>1</v>
+      </c>
+      <c r="T95" s="2" t="str">
+        <f>CONCATENATE(W70,X70)</f>
+        <v>1MATH101</v>
+      </c>
+      <c r="U95" s="2">
+        <v>1</v>
+      </c>
+      <c r="V95" s="2">
+        <v>4</v>
+      </c>
+      <c r="W95" s="14"/>
+      <c r="X95" s="2">
+        <v>8</v>
+      </c>
+      <c r="Y95" s="2" t="str">
+        <f>CONCATENATE(W69,X69)</f>
+        <v>4Study Break</v>
+      </c>
+      <c r="Z95" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA95" s="2">
+        <v>5</v>
+      </c>
+      <c r="AB95" s="47" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="96" spans="4:28" ht="15.75" thickBot="1">
+      <c r="D96" s="3">
+        <v>3</v>
+      </c>
+      <c r="E96" s="3">
+        <v>5</v>
+      </c>
+      <c r="F96" s="3">
+        <v>14</v>
+      </c>
+      <c r="G96" s="3"/>
+      <c r="H96" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I96" s="15"/>
+      <c r="J96" s="16"/>
+      <c r="K96" s="17"/>
+      <c r="L96" s="16"/>
+      <c r="M96" s="18"/>
+      <c r="N96" s="145">
+        <v>6</v>
+      </c>
+      <c r="O96" s="146" t="s">
+        <v>181</v>
+      </c>
+      <c r="P96" s="147">
+        <v>2</v>
+      </c>
+      <c r="Q96" s="146">
+        <v>3</v>
+      </c>
+      <c r="R96" s="51"/>
+      <c r="S96" s="15">
+        <v>1</v>
+      </c>
+      <c r="T96" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="U96" s="17">
+        <v>1</v>
+      </c>
+      <c r="V96" s="16">
+        <v>4</v>
+      </c>
+      <c r="W96" s="18"/>
+      <c r="X96" s="48"/>
+      <c r="Y96" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z96" s="50" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA96" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="AB96" s="51" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="101" spans="8:13">
+      <c r="H101" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J101" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K101" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L101" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M101" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="102" spans="8:13">
+      <c r="H102" s="2">
+        <v>0</v>
+      </c>
+      <c r="I102" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="8:13">
+      <c r="H103" s="2">
+        <v>1</v>
+      </c>
+      <c r="I103" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="8:13">
+      <c r="H104" s="2">
+        <v>1</v>
+      </c>
+      <c r="I104" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="8:13">
+      <c r="H105" s="2">
+        <v>3</v>
+      </c>
+      <c r="I105" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="8:13">
+      <c r="H106" s="2">
+        <v>3</v>
+      </c>
+      <c r="I106" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="8:13">
+      <c r="H107" s="2">
+        <v>5</v>
+      </c>
+      <c r="I107" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="8:13">
+      <c r="H108" s="2">
+        <v>5</v>
+      </c>
+      <c r="I108" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="8:13">
+      <c r="H109" s="2">
+        <v>6</v>
+      </c>
+      <c r="I109" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="8:13">
+      <c r="H110" s="2">
+        <v>6</v>
+      </c>
+      <c r="I110" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="8:13">
+      <c r="H111" s="2">
+        <v>7</v>
+      </c>
+      <c r="I111" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="8:13">
+      <c r="H112" s="2">
+        <v>7</v>
+      </c>
+      <c r="I112" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="8:13">
+      <c r="H113" s="2">
+        <v>8</v>
+      </c>
+      <c r="I113" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="8:13">
+      <c r="H114" s="2">
+        <v>8</v>
+      </c>
+      <c r="I114" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="8:13">
+      <c r="H115" s="2">
+        <v>9</v>
+      </c>
+      <c r="I115" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="8:13">
+      <c r="H116" s="2">
+        <v>10</v>
+      </c>
+      <c r="I116" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="8:13">
+      <c r="H117" s="2">
+        <v>11</v>
+      </c>
+      <c r="I117" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="8:13">
+      <c r="H118" s="2">
+        <v>11</v>
+      </c>
+      <c r="I118" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="8:13">
+      <c r="H119" s="2">
+        <v>12</v>
+      </c>
+      <c r="I119" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="8:13">
+      <c r="H120" s="2">
+        <v>13</v>
+      </c>
+      <c r="I120" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="8:13">
+      <c r="H121" s="2">
+        <v>13</v>
+      </c>
+      <c r="I121" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="8:13">
+      <c r="H122" s="2">
+        <v>14</v>
+      </c>
+      <c r="I122" s="2">
+        <v>3</v>
+      </c>
+      <c r="J122" s="2"/>
+      <c r="K122" s="2"/>
+      <c r="L122" s="2"/>
+      <c r="M122" s="2"/>
+    </row>
+    <row r="123" spans="8:13">
+      <c r="H123" s="2">
+        <v>14</v>
+      </c>
+      <c r="I123" s="2">
+        <v>2</v>
+      </c>
+      <c r="J123" s="2"/>
+      <c r="K123" s="2"/>
+      <c r="L123" s="2"/>
+      <c r="M123" s="2"/>
+    </row>
   </sheetData>
+  <sortState ref="H102:N123">
+    <sortCondition ref="J101"/>
+  </sortState>
+  <mergeCells count="4">
+    <mergeCell ref="I80:M80"/>
+    <mergeCell ref="N80:R80"/>
+    <mergeCell ref="S80:W80"/>
+    <mergeCell ref="X80:AB80"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6253,7 +7872,7 @@
       <selection activeCell="J12" sqref="J12:K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6262,21 +7881,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>151</v>
       </c>
@@ -6287,7 +7907,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -6297,11 +7917,25 @@
       <c r="E2" t="s">
         <v>108</v>
       </c>
-      <c r="H2" s="146" t="s">
+      <c r="H2" s="140" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K2" s="105" t="s">
+        <v>182</v>
+      </c>
+      <c r="M2">
+        <v>33</v>
+      </c>
+      <c r="N2">
+        <f t="shared" ref="N2:N17" si="0">M2/$M$18</f>
+        <v>0.18435754189944134</v>
+      </c>
+      <c r="O2" s="155">
+        <f t="shared" ref="O2:O17" si="1">N2*100</f>
+        <v>18.435754189944134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>109</v>
       </c>
@@ -6311,11 +7945,25 @@
       <c r="E3" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="146" t="s">
+      <c r="H3" s="140" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K3" s="105" t="s">
+        <v>183</v>
+      </c>
+      <c r="M3">
+        <v>20</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>0.11173184357541899</v>
+      </c>
+      <c r="O3" s="148">
+        <f t="shared" si="1"/>
+        <v>11.173184357541899</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>110</v>
       </c>
@@ -6325,11 +7973,25 @@
       <c r="E4" t="s">
         <v>110</v>
       </c>
-      <c r="H4" s="146" t="s">
+      <c r="H4" s="140" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K4" s="105" t="s">
+        <v>184</v>
+      </c>
+      <c r="M4">
+        <v>17</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>9.4972067039106142E-2</v>
+      </c>
+      <c r="O4" s="148">
+        <f t="shared" si="1"/>
+        <v>9.4972067039106136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>111</v>
       </c>
@@ -6339,11 +8001,25 @@
       <c r="E5" t="s">
         <v>143</v>
       </c>
-      <c r="H5" s="146" t="s">
+      <c r="H5" s="140" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K5" s="105" t="s">
+        <v>185</v>
+      </c>
+      <c r="M5">
+        <v>14</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>7.8212290502793297E-2</v>
+      </c>
+      <c r="O5" s="148">
+        <f t="shared" si="1"/>
+        <v>7.8212290502793298</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>112</v>
       </c>
@@ -6353,11 +8029,25 @@
       <c r="E6" t="s">
         <v>130</v>
       </c>
-      <c r="H6" s="146" t="s">
+      <c r="H6" s="140" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K6" s="105" t="s">
+        <v>186</v>
+      </c>
+      <c r="M6">
+        <v>13</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>7.2625698324022353E-2</v>
+      </c>
+      <c r="O6" s="148">
+        <f t="shared" si="1"/>
+        <v>7.2625698324022352</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>113</v>
       </c>
@@ -6367,16 +8057,44 @@
       <c r="E7" t="s">
         <v>113</v>
       </c>
-      <c r="H7" s="146" t="s">
+      <c r="H7" s="140" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H8" s="146" t="s">
+      <c r="K7" s="105" t="s">
+        <v>187</v>
+      </c>
+      <c r="M7">
+        <v>11</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>6.1452513966480445E-2</v>
+      </c>
+      <c r="O7" s="148">
+        <f t="shared" si="1"/>
+        <v>6.1452513966480442</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="H8" s="140" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K8" s="105" t="s">
+        <v>188</v>
+      </c>
+      <c r="M8">
+        <v>10</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>5.5865921787709494E-2</v>
+      </c>
+      <c r="O8" s="148">
+        <f t="shared" si="1"/>
+        <v>5.5865921787709496</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -6386,11 +8104,25 @@
       <c r="E9" t="s">
         <v>114</v>
       </c>
-      <c r="H9" s="146" t="s">
+      <c r="H9" s="140" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K9" s="105" t="s">
+        <v>189</v>
+      </c>
+      <c r="M9">
+        <v>9</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>5.027932960893855E-2</v>
+      </c>
+      <c r="O9" s="148">
+        <f t="shared" si="1"/>
+        <v>5.027932960893855</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>110</v>
       </c>
@@ -6400,11 +8132,25 @@
       <c r="E10" t="s">
         <v>110</v>
       </c>
-      <c r="H10" s="146" t="s">
+      <c r="H10" s="140" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K10" s="105" t="s">
+        <v>190</v>
+      </c>
+      <c r="M10">
+        <v>8</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>4.4692737430167599E-2</v>
+      </c>
+      <c r="O10" s="148">
+        <f t="shared" si="1"/>
+        <v>4.4692737430167595</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>115</v>
       </c>
@@ -6414,11 +8160,25 @@
       <c r="E11" t="s">
         <v>118</v>
       </c>
-      <c r="H11" s="146" t="s">
+      <c r="H11" s="140" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K11" s="105" t="s">
+        <v>191</v>
+      </c>
+      <c r="M11">
+        <v>8</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>4.4692737430167599E-2</v>
+      </c>
+      <c r="O11" s="148">
+        <f t="shared" si="1"/>
+        <v>4.4692737430167595</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>116</v>
       </c>
@@ -6428,11 +8188,25 @@
       <c r="E12" t="s">
         <v>144</v>
       </c>
-      <c r="H12" s="146" t="s">
+      <c r="H12" s="140" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K12" s="105" t="s">
+        <v>192</v>
+      </c>
+      <c r="M12">
+        <v>7</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>3.9106145251396648E-2</v>
+      </c>
+      <c r="O12" s="148">
+        <f t="shared" si="1"/>
+        <v>3.9106145251396649</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>113</v>
       </c>
@@ -6442,19 +8216,47 @@
       <c r="E13" t="s">
         <v>113</v>
       </c>
-      <c r="H13" s="146" t="s">
+      <c r="H13" s="140" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H14" s="146" t="s">
+      <c r="K13" s="105" t="s">
+        <v>193</v>
+      </c>
+      <c r="M13">
+        <v>7</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>3.9106145251396648E-2</v>
+      </c>
+      <c r="O13" s="148">
+        <f t="shared" si="1"/>
+        <v>3.9106145251396649</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="H14" s="140" t="s">
         <v>166</v>
       </c>
       <c r="I14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K14" s="105" t="s">
+        <v>194</v>
+      </c>
+      <c r="M14">
+        <v>6</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>3.3519553072625698E-2</v>
+      </c>
+      <c r="O14" s="148">
+        <f t="shared" si="1"/>
+        <v>3.3519553072625698</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>117</v>
       </c>
@@ -6464,11 +8266,25 @@
       <c r="E15" t="s">
         <v>117</v>
       </c>
-      <c r="H15" s="146" t="s">
+      <c r="H15" s="140" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K15" s="105" t="s">
+        <v>195</v>
+      </c>
+      <c r="M15">
+        <v>6</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>3.3519553072625698E-2</v>
+      </c>
+      <c r="O15" s="148">
+        <f t="shared" si="1"/>
+        <v>3.3519553072625698</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>110</v>
       </c>
@@ -6478,14 +8294,28 @@
       <c r="E16" t="s">
         <v>110</v>
       </c>
-      <c r="H16" s="146" t="s">
+      <c r="H16" s="140" t="s">
         <v>168</v>
       </c>
       <c r="I16">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K16" s="105" t="s">
+        <v>196</v>
+      </c>
+      <c r="M16">
+        <v>5</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>2.7932960893854747E-2</v>
+      </c>
+      <c r="O16" s="148">
+        <f t="shared" si="1"/>
+        <v>2.7932960893854748</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
         <v>118</v>
       </c>
@@ -6495,11 +8325,25 @@
       <c r="E17" t="s">
         <v>126</v>
       </c>
-      <c r="H17" s="146" t="s">
+      <c r="H17" s="140" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K17" s="105" t="s">
+        <v>197</v>
+      </c>
+      <c r="M17">
+        <v>5</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>2.7932960893854747E-2</v>
+      </c>
+      <c r="O17" s="148">
+        <f t="shared" si="1"/>
+        <v>2.7932960893854748</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -6509,11 +8353,18 @@
       <c r="E18" t="s">
         <v>139</v>
       </c>
-      <c r="H18" s="146" t="s">
+      <c r="H18" s="140" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K18" s="105" t="s">
+        <v>198</v>
+      </c>
+      <c r="M18">
+        <f>SUM(M2:M17)</f>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
         <v>120</v>
       </c>
@@ -6523,11 +8374,11 @@
       <c r="E19" t="s">
         <v>140</v>
       </c>
-      <c r="H19" s="146" t="s">
+      <c r="H19" s="140" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
         <v>121</v>
       </c>
@@ -6537,11 +8388,11 @@
       <c r="E20" t="s">
         <v>121</v>
       </c>
-      <c r="H20" s="146" t="s">
+      <c r="H20" s="140" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
         <v>113</v>
       </c>
@@ -6551,16 +8402,16 @@
       <c r="E21" t="s">
         <v>113</v>
       </c>
-      <c r="H21" s="146" t="s">
+      <c r="H21" s="140" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H22" s="146" t="s">
+    <row r="22" spans="1:15">
+      <c r="H22" s="140" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>122</v>
       </c>
@@ -6570,11 +8421,11 @@
       <c r="E23" t="s">
         <v>122</v>
       </c>
-      <c r="H23" s="146" t="s">
+      <c r="H23" s="140" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
         <v>110</v>
       </c>
@@ -6585,7 +8436,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
         <v>123</v>
       </c>
@@ -6596,7 +8447,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15">
       <c r="A26" t="s">
         <v>124</v>
       </c>
@@ -6607,7 +8458,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
         <v>113</v>
       </c>
@@ -6618,7 +8469,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15">
       <c r="A29" t="s">
         <v>125</v>
       </c>
@@ -6629,7 +8480,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15">
       <c r="A30" t="s">
         <v>110</v>
       </c>
@@ -6640,7 +8491,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15">
       <c r="A31" t="s">
         <v>126</v>
       </c>
@@ -6651,7 +8502,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15">
       <c r="A32" t="s">
         <v>127</v>
       </c>
@@ -6662,7 +8513,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>113</v>
       </c>
@@ -6673,7 +8524,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>128</v>
       </c>
@@ -6684,7 +8535,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>110</v>
       </c>
@@ -6695,7 +8546,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>129</v>
       </c>
@@ -6706,7 +8557,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>130</v>
       </c>
@@ -6717,7 +8568,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>131</v>
       </c>
@@ -6728,7 +8579,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>132</v>
       </c>
@@ -6739,7 +8590,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>113</v>
       </c>
@@ -6750,7 +8601,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>133</v>
       </c>
@@ -6761,7 +8612,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>110</v>
       </c>
@@ -6772,7 +8623,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>118</v>
       </c>
@@ -6783,7 +8634,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>134</v>
       </c>
@@ -6794,7 +8645,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>135</v>
       </c>
@@ -6805,7 +8656,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>113</v>
       </c>
@@ -6816,7 +8667,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>136</v>
       </c>
@@ -6827,7 +8678,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>110</v>
       </c>
@@ -6838,7 +8689,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>126</v>
       </c>
@@ -6849,7 +8700,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>112</v>
       </c>
@@ -6860,7 +8711,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>137</v>
       </c>
@@ -6871,7 +8722,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>113</v>
       </c>
@@ -6882,7 +8733,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>138</v>
       </c>

</xml_diff>